<commit_message>
changes path of stimuli
</commit_message>
<xml_diff>
--- a/stimuli_presentation/stim_param.xlsx
+++ b/stimuli_presentation/stim_param.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/monica/Dropbox/NAIST/Teaching/Spring Seminar/2023/SS2023_Physiology/stimuli_presentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF957CC9-4648-B54E-AD93-5835BDF025E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D429EA1-84D1-9241-9D4C-4C7883CF1D77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22520" yWindow="-28300" windowWidth="16040" windowHeight="19160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,10 +28,10 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>../../Videos/duck_video.mp4</t>
+    <t>stimuli/duck_video.mp4</t>
   </si>
   <si>
-    <t>../../Videos/P07s.mp4</t>
+    <t>stimuli/P07s.mp4</t>
   </si>
 </sst>
 </file>
@@ -422,7 +422,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
adds all videos to the stim list
</commit_message>
<xml_diff>
--- a/stimuli_presentation/stim_param.xlsx
+++ b/stimuli_presentation/stim_param.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/monica/Dropbox/NAIST/Teaching/Spring Seminar/2023/SS2023_Physiology/stimuli_presentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D429EA1-84D1-9241-9D4C-4C7883CF1D77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78FCFB62-AD3A-BF4B-8614-F34D85D14705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22520" yWindow="-28300" windowWidth="16040" windowHeight="19160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>movie_name</t>
     <phoneticPr fontId="1"/>
@@ -32,6 +32,123 @@
   </si>
   <si>
     <t>stimuli/P07s.mp4</t>
+  </si>
+  <si>
+    <t>stimuli/Jester.mp4</t>
+  </si>
+  <si>
+    <t>stimuli/Kids_Jack_01.mp4</t>
+  </si>
+  <si>
+    <t>stimuli/Kids_Jack_02.mp4</t>
+  </si>
+  <si>
+    <t>stimuli/Kids_Jack_03.mp4</t>
+  </si>
+  <si>
+    <t>stimuli/Kids_Jack_04.mp4</t>
+  </si>
+  <si>
+    <t>stimuli/Kids_Jack_05.mp4</t>
+  </si>
+  <si>
+    <t>stimuli/Kids_Jack_06.mp4</t>
+  </si>
+  <si>
+    <t>stimuli/Kids_Jack_07.mp4</t>
+  </si>
+  <si>
+    <t>stimuli/Kids_Jack_08.mp4</t>
+  </si>
+  <si>
+    <t>stimuli/Kids_Jack_09.mp4</t>
+  </si>
+  <si>
+    <t>stimuli/Kids_Jack_10.mp4</t>
+  </si>
+  <si>
+    <t>stimuli/Kids_Jack_11.mp4</t>
+  </si>
+  <si>
+    <t>stimuli/Kids_Jack_12.mp4</t>
+  </si>
+  <si>
+    <t>stimuli/Kids_Jack_13.mp4</t>
+  </si>
+  <si>
+    <t>stimuli/Kids_Jack_14.mp4</t>
+  </si>
+  <si>
+    <t>stimuli/Kids_Jack_15.mp4</t>
+  </si>
+  <si>
+    <t>stimuli/Kids_Jack_16.mp4</t>
+  </si>
+  <si>
+    <t>stimuli/Kids_Jack_17.mp4</t>
+  </si>
+  <si>
+    <t>stimuli/Kids_Jack_18.mp4</t>
+  </si>
+  <si>
+    <t>stimuli/Kids_Jack_19.mp4</t>
+  </si>
+  <si>
+    <t>stimuli/Kids_Jack_20.mp4</t>
+  </si>
+  <si>
+    <t>stimuli/Kids_Jack_21.mp4</t>
+  </si>
+  <si>
+    <t>stimuli/Kids_Jack_22.mp4</t>
+  </si>
+  <si>
+    <t>stimuli/Kids_Jack_23.mp4</t>
+  </si>
+  <si>
+    <t>stimuli/Kids_Jack_24.mp4</t>
+  </si>
+  <si>
+    <t>stimuli/Kids_Jack_25.mp4</t>
+  </si>
+  <si>
+    <t>stimuli/Kids_Jack_26.mp4</t>
+  </si>
+  <si>
+    <t>stimuli/Kids_Jack_27.mp4</t>
+  </si>
+  <si>
+    <t>stimuli/Kids_Jack_28.mp4</t>
+  </si>
+  <si>
+    <t>stimuli/Kids_Jack_29.mp4</t>
+  </si>
+  <si>
+    <t>stimuli/P01.mp4</t>
+  </si>
+  <si>
+    <t>stimuli/P02s.mp4</t>
+  </si>
+  <si>
+    <t>stimuli/P03.mp4</t>
+  </si>
+  <si>
+    <t>stimuli/P04.mp4</t>
+  </si>
+  <si>
+    <t>stimuli/P05.mp4</t>
+  </si>
+  <si>
+    <t>stimuli/P06.mp4</t>
+  </si>
+  <si>
+    <t>stimuli/P08.mp4</t>
+  </si>
+  <si>
+    <t>stimuli/P08.mpg</t>
+  </si>
+  <si>
+    <t>stimuli/P09.mp4</t>
   </si>
 </sst>
 </file>
@@ -419,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -442,7 +559,202 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove some videos from the excel
</commit_message>
<xml_diff>
--- a/stimuli_presentation/stim_param.xlsx
+++ b/stimuli_presentation/stim_param.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/monica/Dropbox/NAIST/Teaching/Spring Seminar/2023/SS2023_Physiology/stimuli_presentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78FCFB62-AD3A-BF4B-8614-F34D85D14705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A384A66-F75E-A649-83D0-CD58D3CF7613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22520" yWindow="-28300" windowWidth="16040" windowHeight="19160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="18400" windowHeight="19700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>movie_name</t>
     <phoneticPr fontId="1"/>
@@ -52,21 +52,12 @@
     <t>stimuli/Kids_Jack_05.mp4</t>
   </si>
   <si>
-    <t>stimuli/Kids_Jack_06.mp4</t>
-  </si>
-  <si>
-    <t>stimuli/Kids_Jack_07.mp4</t>
-  </si>
-  <si>
     <t>stimuli/Kids_Jack_08.mp4</t>
   </si>
   <si>
     <t>stimuli/Kids_Jack_09.mp4</t>
   </si>
   <si>
-    <t>stimuli/Kids_Jack_10.mp4</t>
-  </si>
-  <si>
     <t>stimuli/Kids_Jack_11.mp4</t>
   </si>
   <si>
@@ -76,15 +67,6 @@
     <t>stimuli/Kids_Jack_13.mp4</t>
   </si>
   <si>
-    <t>stimuli/Kids_Jack_14.mp4</t>
-  </si>
-  <si>
-    <t>stimuli/Kids_Jack_15.mp4</t>
-  </si>
-  <si>
-    <t>stimuli/Kids_Jack_16.mp4</t>
-  </si>
-  <si>
     <t>stimuli/Kids_Jack_17.mp4</t>
   </si>
   <si>
@@ -115,12 +97,6 @@
     <t>stimuli/Kids_Jack_26.mp4</t>
   </si>
   <si>
-    <t>stimuli/Kids_Jack_27.mp4</t>
-  </si>
-  <si>
-    <t>stimuli/Kids_Jack_28.mp4</t>
-  </si>
-  <si>
     <t>stimuli/Kids_Jack_29.mp4</t>
   </si>
   <si>
@@ -142,13 +118,10 @@
     <t>stimuli/P06.mp4</t>
   </si>
   <si>
-    <t>stimuli/P08.mp4</t>
-  </si>
-  <si>
-    <t>stimuli/P08.mpg</t>
-  </si>
-  <si>
     <t>stimuli/P09.mp4</t>
+  </si>
+  <si>
+    <t>stimuli/PairJack.mp4</t>
   </si>
 </sst>
 </file>
@@ -536,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A42"/>
+  <dimension ref="A1:A33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -699,62 +672,17 @@
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>